<commit_message>
description of #changes results
</commit_message>
<xml_diff>
--- a/articles/aosd_2014/graphs.xlsx
+++ b/articles/aosd_2014/graphs.xlsx
@@ -18616,618 +18616,618 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'commits+d spearman'!$B$1:$B$203</c:f>
+              <c:f>'commits+d spearman'!$A$1:$A$203</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="203"/>
                 <c:pt idx="0">
-                  <c:v>0.00492610837438424</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00985221674876847</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0147783251231527</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0197044334975369</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0246305418719212</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0295566502463054</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0344827586206896</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0394088669950739</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0443349753694581</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0492610837438424</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0541871921182266</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0591133004926108</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0640394088669951</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0689655172413793</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0738916256157635</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0788177339901478</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.083743842364532</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0886699507389162</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0935960591133005</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0985221674876847</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.103448275862069</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.108374384236453</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.113300492610837</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.118226600985222</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.123152709359606</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.12807881773399</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.133004926108374</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.137931034482759</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.142857142857143</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.147783251231527</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.152709359605911</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.157635467980296</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.16256157635468</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.167487684729064</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.172413793103448</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.177339901477833</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.182266009852217</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.187192118226601</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.192118226600985</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.197044334975369</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.201970443349754</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.206896551724138</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.211822660098522</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.216748768472906</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.221674876847291</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.226600985221675</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.231527093596059</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.236453201970443</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.241379310344828</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.246305418719212</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.251231527093596</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.25615763546798</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.261083743842365</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.266009852216749</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.270935960591133</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.275862068965517</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.280788177339901</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.285714285714286</c:v>
+                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.29064039408867</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.295566502463054</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.300492610837438</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.305418719211823</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.310344827586207</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.315270935960591</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.320197044334975</c:v>
+                  <c:v>65.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.32512315270936</c:v>
+                  <c:v>66.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.330049261083744</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.334975369458128</c:v>
+                  <c:v>68.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.339901477832512</c:v>
+                  <c:v>69.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.344827586206897</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.349753694581281</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.354679802955665</c:v>
+                  <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.359605911330049</c:v>
+                  <c:v>73.0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.364532019704433</c:v>
+                  <c:v>74.0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.369458128078818</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.374384236453202</c:v>
+                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.379310344827586</c:v>
+                  <c:v>77.0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.38423645320197</c:v>
+                  <c:v>78.0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.389162561576355</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.394088669950739</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.399014778325123</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.403940886699507</c:v>
+                  <c:v>82.0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.408866995073892</c:v>
+                  <c:v>83.0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.413793103448276</c:v>
+                  <c:v>84.0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.41871921182266</c:v>
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.423645320197044</c:v>
+                  <c:v>86.0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.428571428571429</c:v>
+                  <c:v>87.0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.433497536945813</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.438423645320197</c:v>
+                  <c:v>89.0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.443349753694581</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.448275862068965</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.45320197044335</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.458128078817734</c:v>
+                  <c:v>93.0</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.463054187192118</c:v>
+                  <c:v>94.0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.467980295566502</c:v>
+                  <c:v>95.0</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.472906403940887</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.477832512315271</c:v>
+                  <c:v>97.0</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.482758620689655</c:v>
+                  <c:v>98.0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.487684729064039</c:v>
+                  <c:v>99.0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.492610837438424</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.497536945812808</c:v>
+                  <c:v>101.0</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.502463054187192</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.507389162561576</c:v>
+                  <c:v>103.0</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.512315270935961</c:v>
+                  <c:v>104.0</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.517241379310345</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.522167487684729</c:v>
+                  <c:v>106.0</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.527093596059113</c:v>
+                  <c:v>107.0</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.532019704433498</c:v>
+                  <c:v>108.0</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.536945812807882</c:v>
+                  <c:v>109.0</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.541871921182266</c:v>
+                  <c:v>110.0</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.54679802955665</c:v>
+                  <c:v>111.0</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.551724137931034</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0.556650246305419</c:v>
+                  <c:v>113.0</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.561576354679803</c:v>
+                  <c:v>114.0</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.566502463054187</c:v>
+                  <c:v>115.0</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.571428571428571</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.576354679802956</c:v>
+                  <c:v>117.0</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0.58128078817734</c:v>
+                  <c:v>118.0</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.586206896551724</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.591133004926108</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.596059113300493</c:v>
+                  <c:v>121.0</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.600985221674877</c:v>
+                  <c:v>122.0</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.605911330049261</c:v>
+                  <c:v>123.0</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.610837438423645</c:v>
+                  <c:v>124.0</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0.615763546798029</c:v>
+                  <c:v>125.0</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>0.620689655172414</c:v>
+                  <c:v>126.0</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>0.625615763546798</c:v>
+                  <c:v>127.0</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>0.630541871921182</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0.635467980295566</c:v>
+                  <c:v>129.0</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>0.640394088669951</c:v>
+                  <c:v>130.0</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>0.645320197044335</c:v>
+                  <c:v>131.0</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>0.650246305418719</c:v>
+                  <c:v>132.0</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>0.655172413793103</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>0.660098522167488</c:v>
+                  <c:v>134.0</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0.665024630541872</c:v>
+                  <c:v>135.0</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>0.669950738916256</c:v>
+                  <c:v>136.0</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>0.67487684729064</c:v>
+                  <c:v>137.0</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>0.679802955665024</c:v>
+                  <c:v>138.0</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>0.684729064039409</c:v>
+                  <c:v>139.0</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>0.689655172413793</c:v>
+                  <c:v>140.0</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>0.694581280788177</c:v>
+                  <c:v>141.0</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>0.699507389162561</c:v>
+                  <c:v>142.0</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>0.704433497536946</c:v>
+                  <c:v>143.0</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>0.70935960591133</c:v>
+                  <c:v>144.0</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>0.714285714285714</c:v>
+                  <c:v>145.0</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>0.719211822660098</c:v>
+                  <c:v>146.0</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>0.724137931034483</c:v>
+                  <c:v>147.0</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>0.729064039408867</c:v>
+                  <c:v>148.0</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>0.733990147783251</c:v>
+                  <c:v>149.0</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>0.738916256157635</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0.74384236453202</c:v>
+                  <c:v>151.0</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>0.748768472906404</c:v>
+                  <c:v>152.0</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>0.753694581280788</c:v>
+                  <c:v>153.0</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>0.758620689655172</c:v>
+                  <c:v>154.0</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>0.763546798029557</c:v>
+                  <c:v>155.0</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>0.768472906403941</c:v>
+                  <c:v>156.0</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>0.773399014778325</c:v>
+                  <c:v>157.0</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>0.778325123152709</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>0.783251231527094</c:v>
+                  <c:v>159.0</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>0.788177339901478</c:v>
+                  <c:v>160.0</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>0.793103448275862</c:v>
+                  <c:v>161.0</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>0.798029556650246</c:v>
+                  <c:v>162.0</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>0.802955665024631</c:v>
+                  <c:v>163.0</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>0.807881773399015</c:v>
+                  <c:v>164.0</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>0.812807881773399</c:v>
+                  <c:v>165.0</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>0.817733990147783</c:v>
+                  <c:v>166.0</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>0.822660098522167</c:v>
+                  <c:v>167.0</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>0.827586206896552</c:v>
+                  <c:v>168.0</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>0.832512315270936</c:v>
+                  <c:v>169.0</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>0.83743842364532</c:v>
+                  <c:v>170.0</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>0.842364532019704</c:v>
+                  <c:v>171.0</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>0.847290640394089</c:v>
+                  <c:v>172.0</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>0.852216748768473</c:v>
+                  <c:v>173.0</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>0.857142857142857</c:v>
+                  <c:v>174.0</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>0.862068965517241</c:v>
+                  <c:v>175.0</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>0.866995073891626</c:v>
+                  <c:v>176.0</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>0.87192118226601</c:v>
+                  <c:v>177.0</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>0.876847290640394</c:v>
+                  <c:v>178.0</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>0.881773399014778</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>0.886699507389163</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>0.891625615763547</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>0.896551724137931</c:v>
+                  <c:v>182.0</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>0.901477832512315</c:v>
+                  <c:v>183.0</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.906403940886699</c:v>
+                  <c:v>184.0</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.911330049261084</c:v>
+                  <c:v>185.0</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>0.916256157635468</c:v>
+                  <c:v>186.0</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>0.921182266009852</c:v>
+                  <c:v>187.0</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>0.926108374384236</c:v>
+                  <c:v>188.0</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>0.931034482758621</c:v>
+                  <c:v>189.0</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.935960591133005</c:v>
+                  <c:v>190.0</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>0.940886699507389</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>0.945812807881773</c:v>
+                  <c:v>192.0</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>0.950738916256158</c:v>
+                  <c:v>193.0</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>0.955665024630542</c:v>
+                  <c:v>194.0</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0.960591133004926</c:v>
+                  <c:v>195.0</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.96551724137931</c:v>
+                  <c:v>196.0</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0.970443349753695</c:v>
+                  <c:v>197.0</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0.975369458128079</c:v>
+                  <c:v>198.0</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>0.980295566502463</c:v>
+                  <c:v>199.0</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>0.985221674876847</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0.990147783251231</c:v>
+                  <c:v>201.0</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>0.995073891625616</c:v>
+                  <c:v>202.0</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>1.0</c:v>
+                  <c:v>203.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19867,7 +19867,8 @@
         <c:axId val="-2124575560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="210.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -19890,10 +19891,10 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -43891,7 +43892,7 @@
   <dimension ref="A1:I203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>